<commit_message>
Fixed details of some probe map files
Fixed some xy coordinates
</commit_message>
<xml_diff>
--- a/preprocessing/probeGeometries/NRX_Buzsaki64_8X8_OldPre2016.xlsx
+++ b/preprocessing/probeGeometries/NRX_Buzsaki64_8X8_OldPre2016.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendonw/Dropbox/Code/GitRepos/buzcode/preprocessing/probeGeometries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{BD25ECFD-2EA5-244D-81C3-89DB80B6C138}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{9EB7C620-61B5-BA4D-97FC-2EED7301073B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23660" yWindow="7880" windowWidth="27540" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1660" yWindow="5880" windowWidth="27540" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="40">
   <si>
     <t>SEE DERIVATION BELOW</t>
   </si>
@@ -129,12 +129,24 @@
   <si>
     <t>Omnetics</t>
   </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>X Coordinates (um)</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Y Coordinates (um)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -153,6 +165,12 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -252,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -435,6 +453,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -752,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R70" sqref="R1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -771,7 +793,7 @@
     <col min="14" max="15" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" ht="39" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -783,8 +805,14 @@
       </c>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-    </row>
-    <row r="2" spans="1:16" ht="52" x14ac:dyDescent="0.15">
+      <c r="R1" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="S1" s="61" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="52" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -818,8 +846,14 @@
       <c r="O2" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R2" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="61" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -871,8 +905,14 @@
         <f t="shared" ref="P3:P66" si="8">O3+64</f>
         <v>81</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R3" s="62">
+        <v>0</v>
+      </c>
+      <c r="S3" s="62">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="10">
         <v>2</v>
       </c>
@@ -925,8 +965,14 @@
         <f t="shared" si="8"/>
         <v>86</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R4" s="62">
+        <v>37</v>
+      </c>
+      <c r="S4" s="62">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -979,8 +1025,14 @@
         <f t="shared" si="8"/>
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R5" s="62">
+        <v>4</v>
+      </c>
+      <c r="S5" s="62">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -1033,8 +1085,14 @@
         <f t="shared" si="8"/>
         <v>87</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R6" s="62">
+        <v>33</v>
+      </c>
+      <c r="S6" s="62">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="10">
         <v>5</v>
       </c>
@@ -1087,8 +1145,14 @@
         <f t="shared" si="8"/>
         <v>83</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R7" s="62">
+        <v>8</v>
+      </c>
+      <c r="S7" s="62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -1141,8 +1205,14 @@
         <f t="shared" si="8"/>
         <v>84</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R8" s="62">
+        <v>29</v>
+      </c>
+      <c r="S8" s="62">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="10">
         <v>7</v>
       </c>
@@ -1195,8 +1265,14 @@
         <f t="shared" si="8"/>
         <v>82</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R9" s="62">
+        <v>10</v>
+      </c>
+      <c r="S9" s="62">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="20">
         <v>8</v>
       </c>
@@ -1249,8 +1325,14 @@
         <f t="shared" si="8"/>
         <v>85</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R10" s="62">
+        <v>18.5</v>
+      </c>
+      <c r="S10" s="62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="29">
         <v>9</v>
       </c>
@@ -1303,8 +1385,15 @@
         <f t="shared" si="8"/>
         <v>89</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R11" s="62">
+        <f t="shared" ref="R11:R66" si="10">R3+200</f>
+        <v>200</v>
+      </c>
+      <c r="S11" s="62">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="10">
         <v>10</v>
       </c>
@@ -1357,8 +1446,15 @@
         <f t="shared" si="8"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R12" s="62">
+        <f t="shared" si="10"/>
+        <v>237</v>
+      </c>
+      <c r="S12" s="62">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="10">
         <v>11</v>
       </c>
@@ -1411,8 +1507,15 @@
         <f t="shared" si="8"/>
         <v>88</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R13" s="62">
+        <f t="shared" si="10"/>
+        <v>204</v>
+      </c>
+      <c r="S13" s="62">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -1465,8 +1568,15 @@
         <f t="shared" si="8"/>
         <v>95</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R14" s="62">
+        <f t="shared" si="10"/>
+        <v>233</v>
+      </c>
+      <c r="S14" s="62">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="10">
         <v>13</v>
       </c>
@@ -1519,8 +1629,15 @@
         <f t="shared" si="8"/>
         <v>91</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R15" s="62">
+        <f t="shared" si="10"/>
+        <v>208</v>
+      </c>
+      <c r="S15" s="62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="10">
         <v>14</v>
       </c>
@@ -1573,8 +1690,15 @@
         <f t="shared" si="8"/>
         <v>92</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R16" s="62">
+        <f t="shared" si="10"/>
+        <v>229</v>
+      </c>
+      <c r="S16" s="62">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="10">
         <v>15</v>
       </c>
@@ -1627,8 +1751,15 @@
         <f t="shared" si="8"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R17" s="62">
+        <f t="shared" si="10"/>
+        <v>210</v>
+      </c>
+      <c r="S17" s="62">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="20">
         <v>16</v>
       </c>
@@ -1681,8 +1812,15 @@
         <f t="shared" si="8"/>
         <v>93</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R18" s="62">
+        <f t="shared" si="10"/>
+        <v>218.5</v>
+      </c>
+      <c r="S18" s="62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="29">
         <v>17</v>
       </c>
@@ -1735,8 +1873,15 @@
         <f t="shared" si="8"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R19" s="62">
+        <f t="shared" si="10"/>
+        <v>400</v>
+      </c>
+      <c r="S19" s="62">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="10">
         <v>18</v>
       </c>
@@ -1789,8 +1934,15 @@
         <f t="shared" si="8"/>
         <v>73</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R20" s="62">
+        <f t="shared" si="10"/>
+        <v>437</v>
+      </c>
+      <c r="S20" s="62">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="10">
         <v>19</v>
       </c>
@@ -1843,8 +1995,15 @@
         <f t="shared" si="8"/>
         <v>65</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R21" s="62">
+        <f t="shared" si="10"/>
+        <v>404</v>
+      </c>
+      <c r="S21" s="62">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="10">
         <v>20</v>
       </c>
@@ -1897,8 +2056,15 @@
         <f t="shared" si="8"/>
         <v>72</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R22" s="62">
+        <f t="shared" si="10"/>
+        <v>433</v>
+      </c>
+      <c r="S22" s="62">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="10">
         <v>21</v>
       </c>
@@ -1951,8 +2117,15 @@
         <f t="shared" si="8"/>
         <v>66</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R23" s="62">
+        <f t="shared" si="10"/>
+        <v>408</v>
+      </c>
+      <c r="S23" s="62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="10">
         <v>22</v>
       </c>
@@ -2005,8 +2178,15 @@
         <f t="shared" si="8"/>
         <v>70</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R24" s="62">
+        <f t="shared" si="10"/>
+        <v>429</v>
+      </c>
+      <c r="S24" s="62">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="10">
         <v>23</v>
       </c>
@@ -2059,8 +2239,15 @@
         <f t="shared" si="8"/>
         <v>68</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R25" s="62">
+        <f t="shared" si="10"/>
+        <v>410</v>
+      </c>
+      <c r="S25" s="62">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="20">
         <v>24</v>
       </c>
@@ -2113,8 +2300,15 @@
         <f t="shared" si="8"/>
         <v>69</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R26" s="62">
+        <f t="shared" si="10"/>
+        <v>418.5</v>
+      </c>
+      <c r="S26" s="62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="29">
         <v>25</v>
       </c>
@@ -2167,8 +2361,15 @@
         <f t="shared" si="8"/>
         <v>74</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R27" s="62">
+        <f t="shared" si="10"/>
+        <v>600</v>
+      </c>
+      <c r="S27" s="62">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="10">
         <v>26</v>
       </c>
@@ -2221,8 +2422,15 @@
         <f t="shared" si="8"/>
         <v>67</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R28" s="62">
+        <f t="shared" si="10"/>
+        <v>637</v>
+      </c>
+      <c r="S28" s="62">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="10">
         <v>27</v>
       </c>
@@ -2275,8 +2483,15 @@
         <f t="shared" si="8"/>
         <v>76</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R29" s="62">
+        <f t="shared" si="10"/>
+        <v>604</v>
+      </c>
+      <c r="S29" s="62">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="10">
         <v>28</v>
       </c>
@@ -2329,8 +2544,15 @@
         <f t="shared" si="8"/>
         <v>71</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R30" s="62">
+        <f t="shared" si="10"/>
+        <v>633</v>
+      </c>
+      <c r="S30" s="62">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="10">
         <v>29</v>
       </c>
@@ -2383,8 +2605,15 @@
         <f t="shared" si="8"/>
         <v>77</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R31" s="62">
+        <f t="shared" si="10"/>
+        <v>608</v>
+      </c>
+      <c r="S31" s="62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="10">
         <v>30</v>
       </c>
@@ -2437,8 +2666,15 @@
         <f t="shared" si="8"/>
         <v>75</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R32" s="62">
+        <f t="shared" si="10"/>
+        <v>629</v>
+      </c>
+      <c r="S32" s="62">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="10">
         <v>31</v>
       </c>
@@ -2491,8 +2727,15 @@
         <f t="shared" si="8"/>
         <v>78</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R33" s="62">
+        <f t="shared" si="10"/>
+        <v>610</v>
+      </c>
+      <c r="S33" s="62">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="20">
         <v>32</v>
       </c>
@@ -2545,8 +2788,15 @@
         <f t="shared" si="8"/>
         <v>79</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R34" s="62">
+        <f t="shared" si="10"/>
+        <v>618.5</v>
+      </c>
+      <c r="S34" s="62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="29">
         <v>33</v>
       </c>
@@ -2599,8 +2849,15 @@
         <f t="shared" si="8"/>
         <v>61</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R35" s="62">
+        <f t="shared" si="10"/>
+        <v>800</v>
+      </c>
+      <c r="S35" s="62">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="10">
         <v>34</v>
       </c>
@@ -2653,8 +2910,15 @@
         <f t="shared" si="8"/>
         <v>52</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R36" s="62">
+        <f t="shared" si="10"/>
+        <v>837</v>
+      </c>
+      <c r="S36" s="62">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" s="10">
         <v>35</v>
       </c>
@@ -2707,8 +2971,15 @@
         <f t="shared" si="8"/>
         <v>57</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R37" s="62">
+        <f t="shared" si="10"/>
+        <v>804</v>
+      </c>
+      <c r="S37" s="62">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="10">
         <v>36</v>
       </c>
@@ -2761,8 +3032,15 @@
         <f t="shared" si="8"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R38" s="62">
+        <f t="shared" si="10"/>
+        <v>833</v>
+      </c>
+      <c r="S38" s="62">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="10">
         <v>37</v>
       </c>
@@ -2815,8 +3093,15 @@
         <f t="shared" si="8"/>
         <v>53</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R39" s="62">
+        <f t="shared" si="10"/>
+        <v>808</v>
+      </c>
+      <c r="S39" s="62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="10">
         <v>38</v>
       </c>
@@ -2869,8 +3154,15 @@
         <f t="shared" si="8"/>
         <v>51</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R40" s="62">
+        <f t="shared" si="10"/>
+        <v>829</v>
+      </c>
+      <c r="S40" s="62">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" s="10">
         <v>39</v>
       </c>
@@ -2923,8 +3215,15 @@
         <f t="shared" si="8"/>
         <v>49</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R41" s="62">
+        <f t="shared" si="10"/>
+        <v>810</v>
+      </c>
+      <c r="S41" s="62">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A42" s="20">
         <v>40</v>
       </c>
@@ -2977,8 +3276,15 @@
         <f t="shared" si="8"/>
         <v>48</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R42" s="62">
+        <f t="shared" si="10"/>
+        <v>818.5</v>
+      </c>
+      <c r="S42" s="62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" s="29">
         <v>41</v>
       </c>
@@ -3031,8 +3337,15 @@
         <f t="shared" si="8"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R43" s="62">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="S43" s="62">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" s="10">
         <v>42</v>
       </c>
@@ -3085,8 +3398,15 @@
         <f t="shared" si="8"/>
         <v>62</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R44" s="62">
+        <f t="shared" si="10"/>
+        <v>1037</v>
+      </c>
+      <c r="S44" s="62">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="10">
         <v>43</v>
       </c>
@@ -3139,8 +3459,15 @@
         <f t="shared" si="8"/>
         <v>54</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R45" s="62">
+        <f t="shared" si="10"/>
+        <v>1004</v>
+      </c>
+      <c r="S45" s="62">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A46" s="10">
         <v>44</v>
       </c>
@@ -3193,8 +3520,15 @@
         <f t="shared" si="8"/>
         <v>63</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R46" s="62">
+        <f t="shared" si="10"/>
+        <v>1033</v>
+      </c>
+      <c r="S46" s="62">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" s="10">
         <v>45</v>
       </c>
@@ -3247,8 +3581,15 @@
         <f t="shared" si="8"/>
         <v>56</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R47" s="62">
+        <f t="shared" si="10"/>
+        <v>1008</v>
+      </c>
+      <c r="S47" s="62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A48" s="10">
         <v>46</v>
       </c>
@@ -3301,8 +3642,15 @@
         <f t="shared" si="8"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R48" s="62">
+        <f t="shared" si="10"/>
+        <v>1029</v>
+      </c>
+      <c r="S48" s="62">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A49" s="10">
         <v>47</v>
       </c>
@@ -3355,8 +3703,15 @@
         <f t="shared" si="8"/>
         <v>59</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R49" s="62">
+        <f t="shared" si="10"/>
+        <v>1010</v>
+      </c>
+      <c r="S49" s="62">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A50" s="20">
         <v>48</v>
       </c>
@@ -3409,8 +3764,15 @@
         <f t="shared" si="8"/>
         <v>58</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R50" s="62">
+        <f t="shared" si="10"/>
+        <v>1018.5</v>
+      </c>
+      <c r="S50" s="62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" s="29">
         <v>49</v>
       </c>
@@ -3463,8 +3825,15 @@
         <f t="shared" si="8"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="52" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R51" s="62">
+        <f t="shared" si="10"/>
+        <v>1200</v>
+      </c>
+      <c r="S51" s="62">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A52" s="10">
         <v>50</v>
       </c>
@@ -3517,8 +3886,15 @@
         <f t="shared" si="8"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="53" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R52" s="62">
+        <f t="shared" si="10"/>
+        <v>1237</v>
+      </c>
+      <c r="S52" s="62">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="10">
         <v>51</v>
       </c>
@@ -3571,8 +3947,15 @@
         <f t="shared" si="8"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="54" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R53" s="62">
+        <f t="shared" si="10"/>
+        <v>1204</v>
+      </c>
+      <c r="S53" s="62">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" s="10">
         <v>52</v>
       </c>
@@ -3625,8 +4008,15 @@
         <f t="shared" si="8"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R54" s="62">
+        <f t="shared" si="10"/>
+        <v>1233</v>
+      </c>
+      <c r="S54" s="62">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" s="10">
         <v>53</v>
       </c>
@@ -3679,8 +4069,15 @@
         <f t="shared" si="8"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="56" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R55" s="62">
+        <f t="shared" si="10"/>
+        <v>1208</v>
+      </c>
+      <c r="S55" s="62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A56" s="10">
         <v>54</v>
       </c>
@@ -3733,8 +4130,15 @@
         <f t="shared" si="8"/>
         <v>37</v>
       </c>
-    </row>
-    <row r="57" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R56" s="62">
+        <f t="shared" si="10"/>
+        <v>1229</v>
+      </c>
+      <c r="S56" s="62">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A57" s="10">
         <v>55</v>
       </c>
@@ -3787,8 +4191,15 @@
         <f t="shared" si="8"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="58" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R57" s="62">
+        <f t="shared" si="10"/>
+        <v>1210</v>
+      </c>
+      <c r="S57" s="62">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A58" s="20">
         <v>56</v>
       </c>
@@ -3841,8 +4252,15 @@
         <f t="shared" si="8"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="59" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R58" s="62">
+        <f t="shared" si="10"/>
+        <v>1218.5</v>
+      </c>
+      <c r="S58" s="62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A59" s="29">
         <v>57</v>
       </c>
@@ -3895,8 +4313,15 @@
         <f t="shared" si="8"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R59" s="62">
+        <f t="shared" si="10"/>
+        <v>1400</v>
+      </c>
+      <c r="S59" s="62">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A60" s="10">
         <v>58</v>
       </c>
@@ -3949,8 +4374,15 @@
         <f t="shared" si="8"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="61" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R60" s="62">
+        <f t="shared" si="10"/>
+        <v>1437</v>
+      </c>
+      <c r="S60" s="62">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A61" s="10">
         <v>59</v>
       </c>
@@ -4003,8 +4435,15 @@
         <f t="shared" si="8"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="62" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R61" s="62">
+        <f t="shared" si="10"/>
+        <v>1404</v>
+      </c>
+      <c r="S61" s="62">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A62" s="10">
         <v>60</v>
       </c>
@@ -4057,8 +4496,15 @@
         <f t="shared" si="8"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="63" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R62" s="62">
+        <f t="shared" si="10"/>
+        <v>1433</v>
+      </c>
+      <c r="S62" s="62">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A63" s="10">
         <v>61</v>
       </c>
@@ -4111,8 +4557,15 @@
         <f t="shared" si="8"/>
         <v>42</v>
       </c>
-    </row>
-    <row r="64" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+      <c r="R63" s="62">
+        <f t="shared" si="10"/>
+        <v>1408</v>
+      </c>
+      <c r="S63" s="62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A64" s="10">
         <v>62</v>
       </c>
@@ -4165,8 +4618,15 @@
         <f t="shared" si="8"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="65" spans="1:21" ht="13" x14ac:dyDescent="0.15">
+      <c r="R64" s="62">
+        <f t="shared" si="10"/>
+        <v>1429</v>
+      </c>
+      <c r="S64" s="62">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A65" s="10">
         <v>63</v>
       </c>
@@ -4219,8 +4679,15 @@
         <f t="shared" si="8"/>
         <v>43</v>
       </c>
-    </row>
-    <row r="66" spans="1:21" ht="13" x14ac:dyDescent="0.15">
+      <c r="R65" s="62">
+        <f t="shared" si="10"/>
+        <v>1410</v>
+      </c>
+      <c r="S65" s="62">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" ht="14" x14ac:dyDescent="0.15">
       <c r="A66" s="10">
         <v>64</v>
       </c>
@@ -4272,6 +4739,13 @@
       <c r="P66">
         <f t="shared" si="8"/>
         <v>44</v>
+      </c>
+      <c r="R66" s="62">
+        <f t="shared" si="10"/>
+        <v>1418.5</v>
+      </c>
+      <c r="S66" s="62">
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:21" ht="13" x14ac:dyDescent="0.15">
@@ -4399,7 +4873,7 @@
         <v>36</v>
       </c>
       <c r="E72" s="5">
-        <f t="shared" ref="E72:E87" si="10">A72+1</f>
+        <f t="shared" ref="E72:E87" si="11">A72+1</f>
         <v>17</v>
       </c>
       <c r="G72" s="5">
@@ -4412,7 +4886,7 @@
         <v>63</v>
       </c>
       <c r="J72" s="11">
-        <f t="shared" ref="J72:J87" si="11">G72-1</f>
+        <f t="shared" ref="J72:J87" si="12">G72-1</f>
         <v>14</v>
       </c>
       <c r="L72" s="3"/>
@@ -4421,7 +4895,7 @@
     </row>
     <row r="73" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="11">
-        <f t="shared" ref="A73:A87" si="12">A72+2</f>
+        <f t="shared" ref="A73:A87" si="13">A72+2</f>
         <v>18</v>
       </c>
       <c r="B73" s="48">
@@ -4432,11 +4906,11 @@
         <v>38</v>
       </c>
       <c r="E73" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="G73" s="11">
-        <f t="shared" ref="G73:G79" si="13">G72-2</f>
+        <f t="shared" ref="G73:G79" si="14">G72-2</f>
         <v>13</v>
       </c>
       <c r="H73" s="49">
@@ -4446,7 +4920,7 @@
         <v>61</v>
       </c>
       <c r="J73" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12</v>
       </c>
       <c r="L73" s="3"/>
@@ -4455,7 +4929,7 @@
     </row>
     <row r="74" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>20</v>
       </c>
       <c r="B74" s="48">
@@ -4466,11 +4940,11 @@
         <v>35</v>
       </c>
       <c r="E74" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>21</v>
       </c>
       <c r="G74" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>11</v>
       </c>
       <c r="H74" s="49">
@@ -4480,7 +4954,7 @@
         <v>59</v>
       </c>
       <c r="J74" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="L74" s="3"/>
@@ -4489,7 +4963,7 @@
     </row>
     <row r="75" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>22</v>
       </c>
       <c r="B75" s="48">
@@ -4500,11 +4974,11 @@
         <v>41</v>
       </c>
       <c r="E75" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>23</v>
       </c>
       <c r="G75" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>9</v>
       </c>
       <c r="H75" s="49">
@@ -4514,7 +4988,7 @@
         <v>57</v>
       </c>
       <c r="J75" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="L75" s="3"/>
@@ -4523,7 +4997,7 @@
     </row>
     <row r="76" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>24</v>
       </c>
       <c r="B76" s="48">
@@ -4534,11 +5008,11 @@
         <v>34</v>
       </c>
       <c r="E76" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>25</v>
       </c>
       <c r="G76" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="H76" s="49">
@@ -4548,7 +5022,7 @@
         <v>55</v>
       </c>
       <c r="J76" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="L76" s="3"/>
@@ -4557,7 +5031,7 @@
     </row>
     <row r="77" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>26</v>
       </c>
       <c r="B77" s="48">
@@ -4568,11 +5042,11 @@
         <v>44</v>
       </c>
       <c r="E77" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>27</v>
       </c>
       <c r="G77" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5</v>
       </c>
       <c r="H77" s="49">
@@ -4582,7 +5056,7 @@
         <v>53</v>
       </c>
       <c r="J77" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="L77" s="3"/>
@@ -4591,7 +5065,7 @@
     </row>
     <row r="78" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A78" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>28</v>
       </c>
       <c r="B78" s="48">
@@ -4602,11 +5076,11 @@
         <v>33</v>
       </c>
       <c r="E78" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>29</v>
       </c>
       <c r="G78" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="H78" s="49">
@@ -4616,7 +5090,7 @@
         <v>51</v>
       </c>
       <c r="J78" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="L78" s="3"/>
@@ -4625,7 +5099,7 @@
     </row>
     <row r="79" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>30</v>
       </c>
       <c r="B79" s="48">
@@ -4636,11 +5110,11 @@
         <v>47</v>
       </c>
       <c r="E79" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>31</v>
       </c>
       <c r="G79" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="H79" s="49">
@@ -4650,7 +5124,7 @@
         <v>49</v>
       </c>
       <c r="J79" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L79" s="3"/>
@@ -4659,7 +5133,7 @@
     </row>
     <row r="80" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>32</v>
       </c>
       <c r="B80" s="48">
@@ -4670,7 +5144,7 @@
         <v>18</v>
       </c>
       <c r="E80" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>33</v>
       </c>
       <c r="G80" s="5">
@@ -4683,7 +5157,7 @@
         <v>16</v>
       </c>
       <c r="J80" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>62</v>
       </c>
       <c r="L80" s="3"/>
@@ -4692,7 +5166,7 @@
     </row>
     <row r="81" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>34</v>
       </c>
       <c r="B81" s="48">
@@ -4703,11 +5177,11 @@
         <v>32</v>
       </c>
       <c r="E81" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>35</v>
       </c>
       <c r="G81" s="11">
-        <f t="shared" ref="G81:G87" si="14">G80-2</f>
+        <f t="shared" ref="G81:G87" si="15">G80-2</f>
         <v>61</v>
       </c>
       <c r="H81" s="49">
@@ -4717,7 +5191,7 @@
         <v>14</v>
       </c>
       <c r="J81" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>60</v>
       </c>
       <c r="L81" s="3"/>
@@ -4726,7 +5200,7 @@
     </row>
     <row r="82" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>36</v>
       </c>
       <c r="B82" s="48">
@@ -4737,11 +5211,11 @@
         <v>21</v>
       </c>
       <c r="E82" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>37</v>
       </c>
       <c r="G82" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>59</v>
       </c>
       <c r="H82" s="49">
@@ -4751,7 +5225,7 @@
         <v>12</v>
       </c>
       <c r="J82" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>58</v>
       </c>
       <c r="L82" s="3"/>
@@ -4760,7 +5234,7 @@
     </row>
     <row r="83" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>38</v>
       </c>
       <c r="B83" s="48">
@@ -4771,11 +5245,11 @@
         <v>31</v>
       </c>
       <c r="E83" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>39</v>
       </c>
       <c r="G83" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>57</v>
       </c>
       <c r="H83" s="49">
@@ -4785,7 +5259,7 @@
         <v>10</v>
       </c>
       <c r="J83" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>56</v>
       </c>
       <c r="L83" s="3"/>
@@ -4794,7 +5268,7 @@
     </row>
     <row r="84" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>40</v>
       </c>
       <c r="B84" s="48">
@@ -4805,11 +5279,11 @@
         <v>24</v>
       </c>
       <c r="E84" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>41</v>
       </c>
       <c r="G84" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>55</v>
       </c>
       <c r="H84" s="49">
@@ -4819,7 +5293,7 @@
         <v>8</v>
       </c>
       <c r="J84" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>54</v>
       </c>
       <c r="L84" s="3"/>
@@ -4828,7 +5302,7 @@
     </row>
     <row r="85" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>42</v>
       </c>
       <c r="B85" s="48">
@@ -4839,11 +5313,11 @@
         <v>30</v>
       </c>
       <c r="E85" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>43</v>
       </c>
       <c r="G85" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>53</v>
       </c>
       <c r="H85" s="49">
@@ -4853,7 +5327,7 @@
         <v>6</v>
       </c>
       <c r="J85" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>52</v>
       </c>
       <c r="L85" s="3"/>
@@ -4862,7 +5336,7 @@
     </row>
     <row r="86" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A86" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>44</v>
       </c>
       <c r="B86" s="48">
@@ -4873,11 +5347,11 @@
         <v>27</v>
       </c>
       <c r="E86" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>45</v>
       </c>
       <c r="G86" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>51</v>
       </c>
       <c r="H86" s="49">
@@ -4887,7 +5361,7 @@
         <v>4</v>
       </c>
       <c r="J86" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>50</v>
       </c>
       <c r="L86" s="3"/>
@@ -4896,7 +5370,7 @@
     </row>
     <row r="87" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A87" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>46</v>
       </c>
       <c r="B87" s="48">
@@ -4907,11 +5381,11 @@
         <v>29</v>
       </c>
       <c r="E87" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>47</v>
       </c>
       <c r="G87" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>49</v>
       </c>
       <c r="H87" s="49">
@@ -4921,7 +5395,7 @@
         <v>2</v>
       </c>
       <c r="J87" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>48</v>
       </c>
       <c r="L87" s="3"/>
@@ -5019,7 +5493,7 @@
         <v>35</v>
       </c>
       <c r="D92" s="52" t="str">
-        <f t="shared" ref="D92:D156" si="15">B92</f>
+        <f t="shared" ref="D92:D156" si="16">B92</f>
         <v>Omnetics</v>
       </c>
       <c r="E92" s="5" t="s">
@@ -5031,19 +5505,19 @@
     </row>
     <row r="93" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A93" s="30">
-        <f t="shared" ref="A93:B93" si="16">A72</f>
+        <f t="shared" ref="A93:B93" si="17">A72</f>
         <v>16</v>
       </c>
       <c r="B93" s="53">
+        <f t="shared" si="17"/>
+        <v>37</v>
+      </c>
+      <c r="D93" s="54">
         <f t="shared" si="16"/>
         <v>37</v>
       </c>
-      <c r="D93" s="54">
-        <f t="shared" si="15"/>
-        <v>37</v>
-      </c>
       <c r="E93" s="11">
-        <f t="shared" ref="E93:E156" si="17">A93</f>
+        <f t="shared" ref="E93:E156" si="18">A93</f>
         <v>16</v>
       </c>
       <c r="L93" s="3"/>
@@ -5052,19 +5526,19 @@
     </row>
     <row r="94" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A94" s="21">
-        <f t="shared" ref="A94:B94" si="18">A73</f>
+        <f t="shared" ref="A94:B94" si="19">A73</f>
         <v>18</v>
       </c>
       <c r="B94" s="55">
+        <f t="shared" si="19"/>
+        <v>39</v>
+      </c>
+      <c r="D94" s="56">
+        <f t="shared" si="16"/>
+        <v>39</v>
+      </c>
+      <c r="E94" s="11">
         <f t="shared" si="18"/>
-        <v>39</v>
-      </c>
-      <c r="D94" s="56">
-        <f t="shared" si="15"/>
-        <v>39</v>
-      </c>
-      <c r="E94" s="11">
-        <f t="shared" si="17"/>
         <v>18</v>
       </c>
       <c r="L94" s="3"/>
@@ -5073,19 +5547,19 @@
     </row>
     <row r="95" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="57">
-        <f t="shared" ref="A95:B95" si="19">A74</f>
+        <f t="shared" ref="A95:B95" si="20">A74</f>
         <v>20</v>
       </c>
       <c r="B95" s="58">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>40</v>
       </c>
       <c r="D95" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>40</v>
       </c>
       <c r="E95" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>20</v>
       </c>
       <c r="L95" s="3"/>
@@ -5094,19 +5568,19 @@
     </row>
     <row r="96" spans="1:21" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="57">
-        <f t="shared" ref="A96:B96" si="20">A75</f>
+        <f t="shared" ref="A96:B96" si="21">A75</f>
         <v>22</v>
       </c>
       <c r="B96" s="58">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>42</v>
       </c>
       <c r="D96" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>42</v>
       </c>
       <c r="E96" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>22</v>
       </c>
       <c r="L96" s="3"/>
@@ -5115,19 +5589,19 @@
     </row>
     <row r="97" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A97" s="57">
-        <f t="shared" ref="A97:B97" si="21">A76</f>
+        <f t="shared" ref="A97:B97" si="22">A76</f>
         <v>24</v>
       </c>
       <c r="B97" s="58">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>43</v>
       </c>
       <c r="D97" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43</v>
       </c>
       <c r="E97" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>24</v>
       </c>
       <c r="L97" s="3"/>
@@ -5136,19 +5610,19 @@
     </row>
     <row r="98" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A98" s="57">
-        <f t="shared" ref="A98:B98" si="22">A77</f>
+        <f t="shared" ref="A98:B98" si="23">A77</f>
         <v>26</v>
       </c>
       <c r="B98" s="58">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>45</v>
       </c>
       <c r="D98" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>45</v>
       </c>
       <c r="E98" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>26</v>
       </c>
       <c r="L98" s="3"/>
@@ -5157,19 +5631,19 @@
     </row>
     <row r="99" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A99" s="57">
-        <f t="shared" ref="A99:B99" si="23">A78</f>
+        <f t="shared" ref="A99:B99" si="24">A78</f>
         <v>28</v>
       </c>
       <c r="B99" s="58">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>46</v>
       </c>
       <c r="D99" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>46</v>
       </c>
       <c r="E99" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>28</v>
       </c>
       <c r="L99" s="3"/>
@@ -5178,19 +5652,19 @@
     </row>
     <row r="100" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A100" s="57">
-        <f t="shared" ref="A100:B100" si="24">A79</f>
+        <f t="shared" ref="A100:B100" si="25">A79</f>
         <v>30</v>
       </c>
       <c r="B100" s="58">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>48</v>
       </c>
       <c r="D100" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>48</v>
       </c>
       <c r="E100" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>30</v>
       </c>
       <c r="L100" s="3"/>
@@ -5199,19 +5673,19 @@
     </row>
     <row r="101" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A101" s="57">
-        <f t="shared" ref="A101:B101" si="25">A80</f>
+        <f t="shared" ref="A101:B101" si="26">A80</f>
         <v>32</v>
       </c>
       <c r="B101" s="58">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>17</v>
       </c>
       <c r="D101" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>17</v>
       </c>
       <c r="E101" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>32</v>
       </c>
       <c r="L101" s="3"/>
@@ -5220,19 +5694,19 @@
     </row>
     <row r="102" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A102" s="57">
-        <f t="shared" ref="A102:B102" si="26">A81</f>
+        <f t="shared" ref="A102:B102" si="27">A81</f>
         <v>34</v>
       </c>
       <c r="B102" s="58">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>19</v>
       </c>
       <c r="D102" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>19</v>
       </c>
       <c r="E102" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>34</v>
       </c>
       <c r="L102" s="3"/>
@@ -5241,19 +5715,19 @@
     </row>
     <row r="103" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A103" s="57">
-        <f t="shared" ref="A103:B103" si="27">A82</f>
+        <f t="shared" ref="A103:B103" si="28">A82</f>
         <v>36</v>
       </c>
       <c r="B103" s="58">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>20</v>
       </c>
       <c r="D103" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>20</v>
       </c>
       <c r="E103" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>36</v>
       </c>
       <c r="L103" s="3"/>
@@ -5262,19 +5736,19 @@
     </row>
     <row r="104" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A104" s="57">
-        <f t="shared" ref="A104:B104" si="28">A83</f>
+        <f t="shared" ref="A104:B104" si="29">A83</f>
         <v>38</v>
       </c>
       <c r="B104" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>22</v>
       </c>
       <c r="D104" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>22</v>
       </c>
       <c r="E104" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>38</v>
       </c>
       <c r="L104" s="3"/>
@@ -5283,19 +5757,19 @@
     </row>
     <row r="105" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A105" s="30">
-        <f t="shared" ref="A105:B105" si="29">A84</f>
+        <f t="shared" ref="A105:B105" si="30">A84</f>
         <v>40</v>
       </c>
       <c r="B105" s="59">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>23</v>
       </c>
       <c r="D105" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>23</v>
       </c>
       <c r="E105" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>40</v>
       </c>
       <c r="L105" s="3"/>
@@ -5304,19 +5778,19 @@
     </row>
     <row r="106" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A106" s="11">
-        <f t="shared" ref="A106:B106" si="30">A85</f>
+        <f t="shared" ref="A106:B106" si="31">A85</f>
         <v>42</v>
       </c>
       <c r="B106" s="53">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>25</v>
       </c>
       <c r="D106" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>25</v>
       </c>
       <c r="E106" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>42</v>
       </c>
       <c r="L106" s="3"/>
@@ -5325,19 +5799,19 @@
     </row>
     <row r="107" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A107" s="21">
-        <f t="shared" ref="A107:B107" si="31">A86</f>
+        <f t="shared" ref="A107:B107" si="32">A86</f>
         <v>44</v>
       </c>
       <c r="B107" s="55">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>26</v>
       </c>
       <c r="D107" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>26</v>
       </c>
       <c r="E107" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>44</v>
       </c>
       <c r="L107" s="3"/>
@@ -5346,19 +5820,19 @@
     </row>
     <row r="108" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A108" s="30">
-        <f t="shared" ref="A108:B108" si="32">A87</f>
+        <f t="shared" ref="A108:B108" si="33">A87</f>
         <v>46</v>
       </c>
       <c r="B108" s="59">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>28</v>
       </c>
       <c r="D108" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>28</v>
       </c>
       <c r="E108" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>46</v>
       </c>
       <c r="L108" s="3"/>
@@ -5367,19 +5841,19 @@
     </row>
     <row r="109" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A109" s="11">
-        <f t="shared" ref="A109:A124" si="33">E72</f>
+        <f t="shared" ref="A109:A124" si="34">E72</f>
         <v>17</v>
       </c>
       <c r="B109" s="53">
-        <f t="shared" ref="B109:B124" si="34">D72</f>
+        <f t="shared" ref="B109:B124" si="35">D72</f>
         <v>36</v>
       </c>
       <c r="D109" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>36</v>
       </c>
       <c r="E109" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>17</v>
       </c>
       <c r="L109" s="3"/>
@@ -5388,19 +5862,19 @@
     </row>
     <row r="110" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A110" s="11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>19</v>
       </c>
       <c r="B110" s="53">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>38</v>
       </c>
       <c r="D110" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>38</v>
       </c>
       <c r="E110" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>19</v>
       </c>
       <c r="L110" s="3"/>
@@ -5409,19 +5883,19 @@
     </row>
     <row r="111" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A111" s="11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>21</v>
       </c>
       <c r="B111" s="53">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>35</v>
       </c>
       <c r="D111" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>35</v>
       </c>
       <c r="E111" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>21</v>
       </c>
       <c r="L111" s="3"/>
@@ -5430,19 +5904,19 @@
     </row>
     <row r="112" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A112" s="11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>23</v>
       </c>
       <c r="B112" s="53">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>41</v>
       </c>
       <c r="D112" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>41</v>
       </c>
       <c r="E112" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>23</v>
       </c>
       <c r="L112" s="3"/>
@@ -5451,19 +5925,19 @@
     </row>
     <row r="113" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A113" s="11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>25</v>
       </c>
       <c r="B113" s="53">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>34</v>
       </c>
       <c r="D113" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>34</v>
       </c>
       <c r="E113" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>25</v>
       </c>
       <c r="L113" s="3"/>
@@ -5472,19 +5946,19 @@
     </row>
     <row r="114" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A114" s="11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>27</v>
       </c>
       <c r="B114" s="53">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>44</v>
       </c>
       <c r="D114" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>44</v>
       </c>
       <c r="E114" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>27</v>
       </c>
       <c r="L114" s="3"/>
@@ -5493,19 +5967,19 @@
     </row>
     <row r="115" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A115" s="11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>29</v>
       </c>
       <c r="B115" s="53">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>33</v>
       </c>
       <c r="D115" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>33</v>
       </c>
       <c r="E115" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>29</v>
       </c>
       <c r="L115" s="3"/>
@@ -5514,19 +5988,19 @@
     </row>
     <row r="116" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A116" s="11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>31</v>
       </c>
       <c r="B116" s="53">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>47</v>
       </c>
       <c r="D116" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>47</v>
       </c>
       <c r="E116" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>31</v>
       </c>
       <c r="L116" s="3"/>
@@ -5535,19 +6009,19 @@
     </row>
     <row r="117" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A117" s="11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>33</v>
       </c>
       <c r="B117" s="53">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>18</v>
       </c>
       <c r="D117" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>18</v>
       </c>
       <c r="E117" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>33</v>
       </c>
       <c r="L117" s="3"/>
@@ -5556,19 +6030,19 @@
     </row>
     <row r="118" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A118" s="11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>35</v>
       </c>
       <c r="B118" s="53">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>32</v>
       </c>
       <c r="D118" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>32</v>
       </c>
       <c r="E118" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>35</v>
       </c>
       <c r="L118" s="3"/>
@@ -5577,19 +6051,19 @@
     </row>
     <row r="119" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A119" s="11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>37</v>
       </c>
       <c r="B119" s="53">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>21</v>
       </c>
       <c r="D119" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>21</v>
       </c>
       <c r="E119" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>37</v>
       </c>
       <c r="L119" s="3"/>
@@ -5598,19 +6072,19 @@
     </row>
     <row r="120" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A120" s="11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>39</v>
       </c>
       <c r="B120" s="53">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>31</v>
       </c>
       <c r="D120" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="E120" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>39</v>
       </c>
       <c r="L120" s="3"/>
@@ -5619,19 +6093,19 @@
     </row>
     <row r="121" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A121" s="11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>41</v>
       </c>
       <c r="B121" s="53">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>24</v>
       </c>
       <c r="D121" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>24</v>
       </c>
       <c r="E121" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>41</v>
       </c>
       <c r="L121" s="3"/>
@@ -5640,19 +6114,19 @@
     </row>
     <row r="122" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A122" s="11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>43</v>
       </c>
       <c r="B122" s="53">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>30</v>
       </c>
       <c r="D122" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>30</v>
       </c>
       <c r="E122" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>43</v>
       </c>
       <c r="L122" s="3"/>
@@ -5661,19 +6135,19 @@
     </row>
     <row r="123" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A123" s="11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>45</v>
       </c>
       <c r="B123" s="53">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>27</v>
       </c>
       <c r="D123" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>27</v>
       </c>
       <c r="E123" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>45</v>
       </c>
       <c r="L123" s="3"/>
@@ -5682,19 +6156,19 @@
     </row>
     <row r="124" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A124" s="11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>47</v>
       </c>
       <c r="B124" s="53">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>29</v>
       </c>
       <c r="D124" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>29</v>
       </c>
       <c r="E124" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>47</v>
       </c>
       <c r="L124" s="3"/>
@@ -5703,19 +6177,19 @@
     </row>
     <row r="125" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A125" s="11">
-        <f t="shared" ref="A125:B125" si="35">G72</f>
+        <f t="shared" ref="A125:B125" si="36">G72</f>
         <v>15</v>
       </c>
       <c r="B125" s="53">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>64</v>
       </c>
       <c r="D125" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>64</v>
       </c>
       <c r="E125" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="L125" s="3"/>
@@ -5724,19 +6198,19 @@
     </row>
     <row r="126" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A126" s="11">
-        <f t="shared" ref="A126:B126" si="36">G73</f>
+        <f t="shared" ref="A126:B126" si="37">G73</f>
         <v>13</v>
       </c>
       <c r="B126" s="53">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>62</v>
       </c>
       <c r="D126" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>62</v>
       </c>
       <c r="E126" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
       <c r="L126" s="3"/>
@@ -5745,19 +6219,19 @@
     </row>
     <row r="127" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A127" s="11">
-        <f t="shared" ref="A127:B127" si="37">G74</f>
+        <f t="shared" ref="A127:B127" si="38">G74</f>
         <v>11</v>
       </c>
       <c r="B127" s="53">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>60</v>
       </c>
       <c r="D127" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>60</v>
       </c>
       <c r="E127" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
       <c r="L127" s="3"/>
@@ -5766,19 +6240,19 @@
     </row>
     <row r="128" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A128" s="11">
-        <f t="shared" ref="A128:B128" si="38">G75</f>
+        <f t="shared" ref="A128:B128" si="39">G75</f>
         <v>9</v>
       </c>
       <c r="B128" s="53">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>58</v>
       </c>
       <c r="D128" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>58</v>
       </c>
       <c r="E128" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="L128" s="3"/>
@@ -5787,19 +6261,19 @@
     </row>
     <row r="129" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A129" s="11">
-        <f t="shared" ref="A129:B129" si="39">G76</f>
+        <f t="shared" ref="A129:B129" si="40">G76</f>
         <v>7</v>
       </c>
       <c r="B129" s="53">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>56</v>
       </c>
       <c r="D129" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>56</v>
       </c>
       <c r="E129" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>7</v>
       </c>
       <c r="L129" s="3"/>
@@ -5808,19 +6282,19 @@
     </row>
     <row r="130" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A130" s="11">
-        <f t="shared" ref="A130:B130" si="40">G77</f>
+        <f t="shared" ref="A130:B130" si="41">G77</f>
         <v>5</v>
       </c>
       <c r="B130" s="53">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>54</v>
       </c>
       <c r="D130" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>54</v>
       </c>
       <c r="E130" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="L130" s="3"/>
@@ -5829,19 +6303,19 @@
     </row>
     <row r="131" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A131" s="11">
-        <f t="shared" ref="A131:B131" si="41">G78</f>
+        <f t="shared" ref="A131:B131" si="42">G78</f>
         <v>3</v>
       </c>
       <c r="B131" s="53">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>52</v>
       </c>
       <c r="D131" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>52</v>
       </c>
       <c r="E131" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>3</v>
       </c>
       <c r="L131" s="3"/>
@@ -5850,19 +6324,19 @@
     </row>
     <row r="132" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A132" s="11">
-        <f t="shared" ref="A132:B132" si="42">G79</f>
+        <f t="shared" ref="A132:B132" si="43">G79</f>
         <v>1</v>
       </c>
       <c r="B132" s="53">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>50</v>
       </c>
       <c r="D132" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>50</v>
       </c>
       <c r="E132" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="L132" s="3"/>
@@ -5871,19 +6345,19 @@
     </row>
     <row r="133" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A133" s="11">
-        <f t="shared" ref="A133:B133" si="43">G80</f>
+        <f t="shared" ref="A133:B133" si="44">G80</f>
         <v>63</v>
       </c>
       <c r="B133" s="53">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>15</v>
       </c>
       <c r="D133" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>15</v>
       </c>
       <c r="E133" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>63</v>
       </c>
       <c r="L133" s="3"/>
@@ -5892,19 +6366,19 @@
     </row>
     <row r="134" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A134" s="11">
-        <f t="shared" ref="A134:B134" si="44">G81</f>
+        <f t="shared" ref="A134:B134" si="45">G81</f>
         <v>61</v>
       </c>
       <c r="B134" s="53">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>13</v>
       </c>
       <c r="D134" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>13</v>
       </c>
       <c r="E134" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>61</v>
       </c>
       <c r="L134" s="3"/>
@@ -5913,19 +6387,19 @@
     </row>
     <row r="135" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A135" s="11">
-        <f t="shared" ref="A135:B135" si="45">G82</f>
+        <f t="shared" ref="A135:B135" si="46">G82</f>
         <v>59</v>
       </c>
       <c r="B135" s="53">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>11</v>
       </c>
       <c r="D135" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>11</v>
       </c>
       <c r="E135" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>59</v>
       </c>
       <c r="L135" s="3"/>
@@ -5934,19 +6408,19 @@
     </row>
     <row r="136" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A136" s="11">
-        <f t="shared" ref="A136:B136" si="46">G83</f>
+        <f t="shared" ref="A136:B136" si="47">G83</f>
         <v>57</v>
       </c>
       <c r="B136" s="53">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>9</v>
       </c>
       <c r="D136" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>9</v>
       </c>
       <c r="E136" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>57</v>
       </c>
       <c r="L136" s="3"/>
@@ -5955,19 +6429,19 @@
     </row>
     <row r="137" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A137" s="11">
-        <f t="shared" ref="A137:B137" si="47">G84</f>
+        <f t="shared" ref="A137:B137" si="48">G84</f>
         <v>55</v>
       </c>
       <c r="B137" s="53">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>7</v>
       </c>
       <c r="D137" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="E137" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>55</v>
       </c>
       <c r="L137" s="3"/>
@@ -5976,19 +6450,19 @@
     </row>
     <row r="138" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A138" s="11">
-        <f t="shared" ref="A138:B138" si="48">G85</f>
+        <f t="shared" ref="A138:B138" si="49">G85</f>
         <v>53</v>
       </c>
       <c r="B138" s="53">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>5</v>
       </c>
       <c r="D138" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5</v>
       </c>
       <c r="E138" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>53</v>
       </c>
       <c r="L138" s="3"/>
@@ -5997,19 +6471,19 @@
     </row>
     <row r="139" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A139" s="11">
-        <f t="shared" ref="A139:B139" si="49">G86</f>
+        <f t="shared" ref="A139:B139" si="50">G86</f>
         <v>51</v>
       </c>
       <c r="B139" s="53">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>3</v>
       </c>
       <c r="D139" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
       <c r="E139" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>51</v>
       </c>
       <c r="L139" s="3"/>
@@ -6018,19 +6492,19 @@
     </row>
     <row r="140" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A140" s="11">
-        <f t="shared" ref="A140:B140" si="50">G87</f>
+        <f t="shared" ref="A140:B140" si="51">G87</f>
         <v>49</v>
       </c>
       <c r="B140" s="53">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>1</v>
       </c>
       <c r="D140" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="E140" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>49</v>
       </c>
       <c r="L140" s="3"/>
@@ -6039,19 +6513,19 @@
     </row>
     <row r="141" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A141" s="11">
-        <f t="shared" ref="A141:A156" si="51">J72</f>
+        <f t="shared" ref="A141:A156" si="52">J72</f>
         <v>14</v>
       </c>
       <c r="B141" s="53">
-        <f t="shared" ref="B141:B156" si="52">I72</f>
+        <f t="shared" ref="B141:B156" si="53">I72</f>
         <v>63</v>
       </c>
       <c r="D141" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>63</v>
       </c>
       <c r="E141" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
       <c r="L141" s="3"/>
@@ -6060,19 +6534,19 @@
     </row>
     <row r="142" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A142" s="11">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>12</v>
       </c>
       <c r="B142" s="53">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>61</v>
       </c>
       <c r="D142" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>61</v>
       </c>
       <c r="E142" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="L142" s="3"/>
@@ -6081,19 +6555,19 @@
     </row>
     <row r="143" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A143" s="11">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>10</v>
       </c>
       <c r="B143" s="53">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>59</v>
       </c>
       <c r="D143" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>59</v>
       </c>
       <c r="E143" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>10</v>
       </c>
       <c r="L143" s="3"/>
@@ -6102,19 +6576,19 @@
     </row>
     <row r="144" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A144" s="11">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>8</v>
       </c>
       <c r="B144" s="53">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>57</v>
       </c>
       <c r="D144" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>57</v>
       </c>
       <c r="E144" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8</v>
       </c>
       <c r="L144" s="3"/>
@@ -6123,19 +6597,19 @@
     </row>
     <row r="145" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A145" s="11">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>6</v>
       </c>
       <c r="B145" s="53">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>55</v>
       </c>
       <c r="D145" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>55</v>
       </c>
       <c r="E145" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
       <c r="L145" s="3"/>
@@ -6144,19 +6618,19 @@
     </row>
     <row r="146" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A146" s="11">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>4</v>
       </c>
       <c r="B146" s="53">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>53</v>
       </c>
       <c r="D146" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>53</v>
       </c>
       <c r="E146" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="L146" s="3"/>
@@ -6165,19 +6639,19 @@
     </row>
     <row r="147" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A147" s="11">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="B147" s="53">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>51</v>
       </c>
       <c r="D147" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>51</v>
       </c>
       <c r="E147" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="L147" s="3"/>
@@ -6186,19 +6660,19 @@
     </row>
     <row r="148" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A148" s="11">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="B148" s="53">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>49</v>
       </c>
       <c r="D148" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>49</v>
       </c>
       <c r="E148" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L148" s="3"/>
@@ -6207,19 +6681,19 @@
     </row>
     <row r="149" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A149" s="11">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>62</v>
       </c>
       <c r="B149" s="53">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>16</v>
       </c>
       <c r="D149" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>16</v>
       </c>
       <c r="E149" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>62</v>
       </c>
       <c r="L149" s="3"/>
@@ -6228,19 +6702,19 @@
     </row>
     <row r="150" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A150" s="11">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>60</v>
       </c>
       <c r="B150" s="53">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>14</v>
       </c>
       <c r="D150" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>14</v>
       </c>
       <c r="E150" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>60</v>
       </c>
       <c r="L150" s="3"/>
@@ -6249,19 +6723,19 @@
     </row>
     <row r="151" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A151" s="11">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>58</v>
       </c>
       <c r="B151" s="53">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>12</v>
       </c>
       <c r="D151" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>12</v>
       </c>
       <c r="E151" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>58</v>
       </c>
       <c r="L151" s="3"/>
@@ -6270,19 +6744,19 @@
     </row>
     <row r="152" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A152" s="11">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>56</v>
       </c>
       <c r="B152" s="53">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>10</v>
       </c>
       <c r="D152" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>10</v>
       </c>
       <c r="E152" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>56</v>
       </c>
       <c r="L152" s="3"/>
@@ -6291,19 +6765,19 @@
     </row>
     <row r="153" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A153" s="11">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>54</v>
       </c>
       <c r="B153" s="53">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>8</v>
       </c>
       <c r="D153" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="E153" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>54</v>
       </c>
       <c r="L153" s="3"/>
@@ -6312,19 +6786,19 @@
     </row>
     <row r="154" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A154" s="11">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>52</v>
       </c>
       <c r="B154" s="53">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>6</v>
       </c>
       <c r="D154" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="E154" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>52</v>
       </c>
       <c r="L154" s="3"/>
@@ -6333,19 +6807,19 @@
     </row>
     <row r="155" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A155" s="11">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>50</v>
       </c>
       <c r="B155" s="53">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>4</v>
       </c>
       <c r="D155" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="E155" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>50</v>
       </c>
       <c r="L155" s="3"/>
@@ -6354,19 +6828,19 @@
     </row>
     <row r="156" spans="1:15" ht="13" x14ac:dyDescent="0.15">
       <c r="A156" s="11">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>48</v>
       </c>
       <c r="B156" s="53">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>2</v>
       </c>
       <c r="D156" s="56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="E156" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>48</v>
       </c>
       <c r="L156" s="3"/>

</xml_diff>